<commit_message>
Added Domain + Controller
Added Domain File and Controller File
</commit_message>
<xml_diff>
--- a/docs/exercise/GradedExercise.xlsx
+++ b/docs/exercise/GradedExercise.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas\Documents\GitHub\hs17-bewertete-uebung-jelenakreuzer\docs\exercise\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16220" yWindow="28800" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="16215" yWindow="28800" windowWidth="25365" windowHeight="15825" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="TOTAL_POINTS">Sheet1!$I$32</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -162,11 +167,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,6 +221,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -245,7 +256,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -253,14 +264,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -589,16 +609,16 @@
   <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.875" customWidth="1"/>
+    <col min="3" max="3" width="14.625" customWidth="1"/>
+    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9">
@@ -634,7 +654,7 @@
       <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="7">
         <v>5</v>
       </c>
     </row>
@@ -645,7 +665,7 @@
       <c r="E5" t="s">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="7">
         <v>15</v>
       </c>
     </row>
@@ -672,7 +692,7 @@
       <c r="E8" t="s">
         <v>2</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="7">
         <v>2</v>
       </c>
     </row>
@@ -683,7 +703,7 @@
       <c r="E9" t="s">
         <v>3</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="7">
         <v>2</v>
       </c>
     </row>
@@ -694,7 +714,7 @@
       <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="7">
         <v>3</v>
       </c>
     </row>
@@ -747,7 +767,7 @@
       <c r="E15" t="s">
         <v>10</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="7">
         <v>5</v>
       </c>
     </row>
@@ -769,7 +789,7 @@
       <c r="E17" t="s">
         <v>12</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="7">
         <v>2</v>
       </c>
     </row>
@@ -780,7 +800,7 @@
       <c r="E18" t="s">
         <v>11</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="7">
         <v>2</v>
       </c>
     </row>

</xml_diff>